<commit_message>
optimised v1 chart config
</commit_message>
<xml_diff>
--- a/price_app/scripts/momentum_analysis/momentum_analysis_output.xlsx
+++ b/price_app/scripts/momentum_analysis/momentum_analysis_output.xlsx
@@ -850,41 +850,41 @@
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>09:16:24</t>
+          <t>09:16:11</t>
         </is>
       </c>
       <c r="C2" s="2" t="inlineStr">
         <is>
-          <t>09:17:01</t>
+          <t>09:16:23</t>
         </is>
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>up</t>
+          <t>down</t>
         </is>
       </c>
-      <c r="E2" t="n">
-        <v>25924.9</v>
-      </c>
-      <c r="F2" t="n">
-        <v>25919.6</v>
-      </c>
-      <c r="G2" t="n">
-        <v>-5.3</v>
-      </c>
-      <c r="I2" t="inlineStr">
+      <c r="E2" s="0" t="n">
+        <v>25913.35</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>25923.65</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>-10.3</v>
+      </c>
+      <c r="I2" s="0" t="inlineStr">
         <is>
-          <t>-10 &lt;-&gt; -5</t>
+          <t>-15 &lt;-&gt; -10</t>
         </is>
       </c>
-      <c r="J2" t="n">
-        <v>5</v>
-      </c>
-      <c r="K2" t="n">
-        <v>5</v>
-      </c>
-      <c r="L2" t="n">
-        <v>50</v>
+      <c r="J2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="K2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="L2" s="0" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="3" ht="15.75" customHeight="1" s="8">
@@ -895,12 +895,12 @@
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>09:17:03</t>
+          <t>09:18:30</t>
         </is>
       </c>
       <c r="C3" s="4" t="inlineStr">
         <is>
-          <t>09:17:10</t>
+          <t>09:19:16</t>
         </is>
       </c>
       <c r="D3" s="2" t="inlineStr">
@@ -908,28 +908,28 @@
           <t>down</t>
         </is>
       </c>
-      <c r="E3" t="n">
-        <v>25916.55</v>
-      </c>
-      <c r="F3" t="n">
-        <v>25921.8</v>
-      </c>
-      <c r="G3" t="n">
-        <v>-5.25</v>
-      </c>
-      <c r="I3" t="inlineStr">
+      <c r="E3" s="0" t="n">
+        <v>25911.3</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>25922.05</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>-10.75</v>
+      </c>
+      <c r="I3" s="0" t="inlineStr">
         <is>
-          <t>-5 &lt;-&gt; 0</t>
+          <t>-10 &lt;-&gt; -5</t>
         </is>
       </c>
-      <c r="J3" t="n">
-        <v>2</v>
-      </c>
-      <c r="K3" t="n">
-        <v>7</v>
-      </c>
-      <c r="L3" t="n">
-        <v>70</v>
+      <c r="J3" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="L3" s="0" t="n">
+        <v>45</v>
       </c>
     </row>
     <row r="4" ht="15.75" customHeight="1" s="8">
@@ -940,12 +940,12 @@
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>09:18:39</t>
+          <t>09:19:44</t>
         </is>
       </c>
       <c r="C4" s="2" t="inlineStr">
         <is>
-          <t>09:18:45</t>
+          <t>09:20:17</t>
         </is>
       </c>
       <c r="D4" s="2" t="inlineStr">
@@ -953,28 +953,28 @@
           <t>up</t>
         </is>
       </c>
-      <c r="E4" t="n">
-        <v>25919.55</v>
-      </c>
-      <c r="F4" t="n">
-        <v>25913.45</v>
-      </c>
-      <c r="G4" t="n">
-        <v>-6.1</v>
-      </c>
-      <c r="I4" t="inlineStr">
+      <c r="E4" s="0" t="n">
+        <v>25934.5</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>25924.2</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>-10.3</v>
+      </c>
+      <c r="I4" s="0" t="inlineStr">
         <is>
-          <t>0 &lt;-&gt; 5</t>
+          <t>-5 &lt;-&gt; 0</t>
         </is>
       </c>
-      <c r="J4" t="n">
-        <v>1</v>
-      </c>
-      <c r="K4" t="n">
-        <v>8</v>
-      </c>
-      <c r="L4" t="n">
-        <v>80</v>
+      <c r="J4" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>74</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1" s="8">
@@ -985,41 +985,41 @@
       </c>
       <c r="B5" s="2" t="inlineStr">
         <is>
-          <t>09:18:46</t>
+          <t>09:22:41</t>
         </is>
       </c>
       <c r="C5" s="2" t="inlineStr">
         <is>
-          <t>09:18:58</t>
+          <t>09:24:59</t>
         </is>
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>down</t>
+          <t>up</t>
         </is>
       </c>
-      <c r="E5" t="n">
-        <v>25913.1</v>
-      </c>
-      <c r="F5" t="n">
-        <v>25917.1</v>
-      </c>
-      <c r="G5" t="n">
-        <v>-4</v>
-      </c>
-      <c r="I5" t="inlineStr">
+      <c r="E5" s="0" t="n">
+        <v>25928.4</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>25926.4</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>-2</v>
+      </c>
+      <c r="I5" s="0" t="inlineStr">
         <is>
-          <t>5 &lt;-&gt; 10</t>
+          <t>0 &lt;-&gt; 5</t>
         </is>
       </c>
-      <c r="J5" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" t="n">
-        <v>8</v>
-      </c>
-      <c r="L5" t="n">
-        <v>80</v>
+      <c r="J5" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>84</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1" s="8">
@@ -1030,12 +1030,12 @@
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>09:20:16</t>
+          <t>09:27:00</t>
         </is>
       </c>
       <c r="C6" s="2" t="inlineStr">
         <is>
-          <t>09:20:54</t>
+          <t>09:28:46</t>
         </is>
       </c>
       <c r="D6" s="2" t="inlineStr">
@@ -1043,27 +1043,27 @@
           <t>down</t>
         </is>
       </c>
-      <c r="E6" t="n">
-        <v>25925.05</v>
-      </c>
-      <c r="F6" t="n">
-        <v>25922.95</v>
-      </c>
-      <c r="G6" t="n">
-        <v>2.1</v>
-      </c>
-      <c r="I6" t="inlineStr">
+      <c r="E6" s="0" t="n">
+        <v>25922.25</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>25928.35</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>-6.1</v>
+      </c>
+      <c r="I6" s="0" t="inlineStr">
         <is>
-          <t>10 &lt;-&gt; 15</t>
+          <t>5 &lt;-&gt; 10</t>
         </is>
       </c>
-      <c r="J6" t="n">
-        <v>1</v>
-      </c>
-      <c r="K6" t="n">
-        <v>9</v>
-      </c>
-      <c r="L6" t="n">
+      <c r="J6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="L6" s="0" t="n">
         <v>90</v>
       </c>
     </row>
@@ -1075,41 +1075,41 @@
       </c>
       <c r="B7" s="2" t="inlineStr">
         <is>
-          <t>09:21:03</t>
+          <t>09:29:24</t>
         </is>
       </c>
       <c r="C7" s="2" t="inlineStr">
         <is>
-          <t>09:21:12</t>
+          <t>09:30:16</t>
         </is>
       </c>
       <c r="D7" s="2" t="inlineStr">
         <is>
-          <t>down</t>
+          <t>up</t>
         </is>
       </c>
-      <c r="E7" t="n">
-        <v>25916.65</v>
-      </c>
-      <c r="F7" t="n">
-        <v>25921.75</v>
-      </c>
-      <c r="G7" t="n">
-        <v>-5.1</v>
-      </c>
-      <c r="I7" t="inlineStr">
+      <c r="E7" s="0" t="n">
+        <v>25931.75</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>25926.3</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>-5.45</v>
+      </c>
+      <c r="I7" s="0" t="inlineStr">
         <is>
-          <t>15 &lt;-&gt; 20</t>
+          <t>10 &lt;-&gt; 15</t>
         </is>
       </c>
-      <c r="J7" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" t="n">
-        <v>9</v>
-      </c>
-      <c r="L7" t="n">
-        <v>90</v>
+      <c r="J7" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <v>97</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1" s="8">
@@ -1120,41 +1120,41 @@
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
-          <t>10:42:07</t>
+          <t>09:35:38</t>
         </is>
       </c>
       <c r="C8" s="2" t="inlineStr">
         <is>
-          <t>10:42:23</t>
+          <t>09:39:02</t>
         </is>
       </c>
       <c r="D8" s="2" t="inlineStr">
         <is>
-          <t>down</t>
+          <t>up</t>
         </is>
       </c>
-      <c r="E8" t="n">
-        <v>25954.15</v>
-      </c>
-      <c r="F8" t="n">
-        <v>25960.65</v>
-      </c>
-      <c r="G8" t="n">
-        <v>-6.5</v>
-      </c>
-      <c r="I8" t="inlineStr">
+      <c r="E8" s="0" t="n">
+        <v>25939.35</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>25935.7</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>-3.65</v>
+      </c>
+      <c r="I8" s="0" t="inlineStr">
         <is>
-          <t>20 &lt;-&gt; 25</t>
+          <t>15 &lt;-&gt; 20</t>
         </is>
       </c>
-      <c r="J8" t="n">
-        <v>0</v>
-      </c>
-      <c r="K8" t="n">
-        <v>9</v>
-      </c>
-      <c r="L8" t="n">
-        <v>90</v>
+      <c r="J8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="L8" s="0" t="n">
+        <v>100</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1" s="8">
@@ -1165,12 +1165,12 @@
       </c>
       <c r="B9" s="2" t="inlineStr">
         <is>
-          <t>15:01:24</t>
+          <t>09:42:49</t>
         </is>
       </c>
       <c r="C9" s="2" t="inlineStr">
         <is>
-          <t>15:01:24</t>
+          <t>09:49:00</t>
         </is>
       </c>
       <c r="D9" s="2" t="inlineStr">
@@ -1178,29 +1178,19 @@
           <t>up</t>
         </is>
       </c>
-      <c r="E9" t="n">
-        <v>25985.95</v>
-      </c>
-      <c r="F9" t="n">
-        <v>26000.25</v>
-      </c>
-      <c r="G9" t="n">
-        <v>14.3</v>
-      </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>25 &lt;-&gt; 30</t>
-        </is>
-      </c>
-      <c r="J9" t="n">
-        <v>1</v>
-      </c>
-      <c r="K9" t="n">
-        <v>10</v>
-      </c>
-      <c r="L9" t="n">
-        <v>100</v>
-      </c>
+      <c r="E9" s="0" t="n">
+        <v>25941.7</v>
+      </c>
+      <c r="F9" s="0" t="n">
+        <v>25957.3</v>
+      </c>
+      <c r="G9" s="0" t="n">
+        <v>15.6</v>
+      </c>
+      <c r="I9" s="0" t="n"/>
+      <c r="J9" s="0" t="n"/>
+      <c r="K9" s="0" t="n"/>
+      <c r="L9" s="0" t="n"/>
     </row>
     <row r="10" ht="15.75" customHeight="1" s="8">
       <c r="A10" s="2" t="inlineStr">
@@ -1210,12 +1200,12 @@
       </c>
       <c r="B10" s="2" t="inlineStr">
         <is>
-          <t>15:01:24</t>
+          <t>10:00:57</t>
         </is>
       </c>
       <c r="C10" s="2" t="inlineStr">
         <is>
-          <t>15:01:24</t>
+          <t>10:05:05</t>
         </is>
       </c>
       <c r="D10" s="2" t="inlineStr">
@@ -1223,14 +1213,14 @@
           <t>down</t>
         </is>
       </c>
-      <c r="E10" t="n">
-        <v>25998.45</v>
-      </c>
-      <c r="F10" t="n">
-        <v>25970.65</v>
-      </c>
-      <c r="G10" t="n">
-        <v>27.8</v>
+      <c r="E10" s="0" t="n">
+        <v>25960.75</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>25961.4</v>
+      </c>
+      <c r="G10" s="0" t="n">
+        <v>-0.65</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1" s="8">
@@ -1241,12 +1231,12 @@
       </c>
       <c r="B11" s="2" t="inlineStr">
         <is>
-          <t>15:01:26</t>
+          <t>10:06:42</t>
         </is>
       </c>
       <c r="C11" s="2" t="inlineStr">
         <is>
-          <t>15:01:26</t>
+          <t>10:09:55</t>
         </is>
       </c>
       <c r="D11" s="2" t="inlineStr">
@@ -1254,141 +1244,666 @@
           <t>up</t>
         </is>
       </c>
-      <c r="E11" t="n">
-        <v>25953.8</v>
-      </c>
-      <c r="F11" t="n">
-        <v>25952.3</v>
-      </c>
-      <c r="G11" t="n">
+      <c r="E11" s="0" t="n">
+        <v>25967.55</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>25968.25</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="12" ht="15.75" customHeight="1" s="8">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>2024-09-24</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="inlineStr">
+        <is>
+          <t>10:11:33</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="inlineStr">
+        <is>
+          <t>10:15:02</t>
+        </is>
+      </c>
+      <c r="D12" s="2" t="inlineStr">
+        <is>
+          <t>down</t>
+        </is>
+      </c>
+      <c r="E12" t="n">
+        <v>25958.2</v>
+      </c>
+      <c r="F12" t="n">
+        <v>25958.45</v>
+      </c>
+      <c r="G12" t="n">
+        <v>-0.25</v>
+      </c>
+    </row>
+    <row r="13" ht="15.75" customHeight="1" s="8">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>2024-09-24</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="inlineStr">
+        <is>
+          <t>10:18:11</t>
+        </is>
+      </c>
+      <c r="C13" s="2" t="inlineStr">
+        <is>
+          <t>10:29:51</t>
+        </is>
+      </c>
+      <c r="D13" s="2" t="inlineStr">
+        <is>
+          <t>up</t>
+        </is>
+      </c>
+      <c r="E13" t="n">
+        <v>25964.6</v>
+      </c>
+      <c r="F13" t="n">
+        <v>25971.3</v>
+      </c>
+      <c r="G13" t="n">
+        <v>6.7</v>
+      </c>
+    </row>
+    <row r="14" ht="15.75" customHeight="1" s="8">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>2024-09-24</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="inlineStr">
+        <is>
+          <t>10:42:16</t>
+        </is>
+      </c>
+      <c r="C14" s="2" t="inlineStr">
+        <is>
+          <t>10:49:30</t>
+        </is>
+      </c>
+      <c r="D14" s="2" t="inlineStr">
+        <is>
+          <t>down</t>
+        </is>
+      </c>
+      <c r="E14" t="n">
+        <v>25957.65</v>
+      </c>
+      <c r="F14" t="n">
+        <v>25947.65</v>
+      </c>
+      <c r="G14" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" ht="15.75" customHeight="1" s="8">
+      <c r="A15" s="2" t="inlineStr">
+        <is>
+          <t>2024-09-24</t>
+        </is>
+      </c>
+      <c r="B15" s="2" t="inlineStr">
+        <is>
+          <t>10:59:25</t>
+        </is>
+      </c>
+      <c r="C15" s="2" t="inlineStr">
+        <is>
+          <t>11:02:14</t>
+        </is>
+      </c>
+      <c r="D15" s="2" t="inlineStr">
+        <is>
+          <t>up</t>
+        </is>
+      </c>
+      <c r="E15" t="n">
+        <v>25956.85</v>
+      </c>
+      <c r="F15" t="n">
+        <v>25951.7</v>
+      </c>
+      <c r="G15" t="n">
+        <v>-5.15</v>
+      </c>
+    </row>
+    <row r="16" ht="15.75" customHeight="1" s="8">
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t>2024-09-24</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="inlineStr">
+        <is>
+          <t>11:04:39</t>
+        </is>
+      </c>
+      <c r="C16" s="2" t="inlineStr">
+        <is>
+          <t>11:08:37</t>
+        </is>
+      </c>
+      <c r="D16" s="2" t="inlineStr">
+        <is>
+          <t>down</t>
+        </is>
+      </c>
+      <c r="E16" t="n">
+        <v>25945.85</v>
+      </c>
+      <c r="F16" t="n">
+        <v>25954.15</v>
+      </c>
+      <c r="G16" t="n">
+        <v>-8.300000000000001</v>
+      </c>
+    </row>
+    <row r="17" ht="15.75" customHeight="1" s="8">
+      <c r="A17" s="2" t="inlineStr">
+        <is>
+          <t>2024-09-24</t>
+        </is>
+      </c>
+      <c r="B17" s="2" t="inlineStr">
+        <is>
+          <t>11:12:54</t>
+        </is>
+      </c>
+      <c r="C17" s="2" t="inlineStr">
+        <is>
+          <t>11:13:57</t>
+        </is>
+      </c>
+      <c r="D17" s="2" t="inlineStr">
+        <is>
+          <t>down</t>
+        </is>
+      </c>
+      <c r="E17" t="n">
+        <v>25948.4</v>
+      </c>
+      <c r="F17" t="n">
+        <v>25954.8</v>
+      </c>
+      <c r="G17" t="n">
+        <v>-6.4</v>
+      </c>
+    </row>
+    <row r="18" ht="15.75" customHeight="1" s="8">
+      <c r="A18" s="2" t="inlineStr">
+        <is>
+          <t>2024-09-24</t>
+        </is>
+      </c>
+      <c r="B18" s="2" t="inlineStr">
+        <is>
+          <t>11:15:27</t>
+        </is>
+      </c>
+      <c r="C18" s="2" t="inlineStr">
+        <is>
+          <t>11:29:06</t>
+        </is>
+      </c>
+      <c r="D18" s="2" t="inlineStr">
+        <is>
+          <t>down</t>
+        </is>
+      </c>
+      <c r="E18" t="n">
+        <v>25944.6</v>
+      </c>
+      <c r="F18" t="n">
+        <v>25930.5</v>
+      </c>
+      <c r="G18" t="n">
+        <v>14.1</v>
+      </c>
+    </row>
+    <row r="19" ht="15.75" customHeight="1" s="8">
+      <c r="A19" s="2" t="inlineStr">
+        <is>
+          <t>2024-09-24</t>
+        </is>
+      </c>
+      <c r="B19" s="2" t="inlineStr">
+        <is>
+          <t>11:53:48</t>
+        </is>
+      </c>
+      <c r="C19" s="2" t="inlineStr">
+        <is>
+          <t>12:00:59</t>
+        </is>
+      </c>
+      <c r="D19" s="2" t="inlineStr">
+        <is>
+          <t>down</t>
+        </is>
+      </c>
+      <c r="E19" t="n">
+        <v>25919.6</v>
+      </c>
+      <c r="F19" t="n">
+        <v>25915.9</v>
+      </c>
+      <c r="G19" t="n">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="20" ht="15.75" customHeight="1" s="8">
+      <c r="A20" s="2" t="inlineStr">
+        <is>
+          <t>2024-09-24</t>
+        </is>
+      </c>
+      <c r="B20" s="2" t="inlineStr">
+        <is>
+          <t>12:16:58</t>
+        </is>
+      </c>
+      <c r="C20" s="2" t="inlineStr">
+        <is>
+          <t>12:27:54</t>
+        </is>
+      </c>
+      <c r="D20" s="2" t="inlineStr">
+        <is>
+          <t>up</t>
+        </is>
+      </c>
+      <c r="E20" t="n">
+        <v>25931.35</v>
+      </c>
+      <c r="F20" t="n">
+        <v>25935.9</v>
+      </c>
+      <c r="G20" t="n">
+        <v>4.55</v>
+      </c>
+    </row>
+    <row r="21" ht="15.75" customHeight="1" s="8">
+      <c r="A21" s="2" t="inlineStr">
+        <is>
+          <t>2024-09-24</t>
+        </is>
+      </c>
+      <c r="B21" s="2" t="inlineStr">
+        <is>
+          <t>12:28:58</t>
+        </is>
+      </c>
+      <c r="C21" s="2" t="inlineStr">
+        <is>
+          <t>12:29:43</t>
+        </is>
+      </c>
+      <c r="D21" s="2" t="inlineStr">
+        <is>
+          <t>down</t>
+        </is>
+      </c>
+      <c r="E21" t="n">
+        <v>25932.75</v>
+      </c>
+      <c r="F21" t="n">
+        <v>25939.55</v>
+      </c>
+      <c r="G21" t="n">
+        <v>-6.8</v>
+      </c>
+    </row>
+    <row r="22" ht="15.75" customHeight="1" s="8">
+      <c r="A22" s="2" t="inlineStr">
+        <is>
+          <t>2024-09-24</t>
+        </is>
+      </c>
+      <c r="B22" s="2" t="inlineStr">
+        <is>
+          <t>12:35:07</t>
+        </is>
+      </c>
+      <c r="C22" s="2" t="inlineStr">
+        <is>
+          <t>13:10:33</t>
+        </is>
+      </c>
+      <c r="D22" s="2" t="inlineStr">
+        <is>
+          <t>up</t>
+        </is>
+      </c>
+      <c r="E22" t="n">
+        <v>25947.25</v>
+      </c>
+      <c r="F22" t="n">
+        <v>25957.6</v>
+      </c>
+      <c r="G22" t="n">
+        <v>10.35</v>
+      </c>
+    </row>
+    <row r="23" ht="15.75" customHeight="1" s="8">
+      <c r="A23" s="2" t="inlineStr">
+        <is>
+          <t>2024-09-24</t>
+        </is>
+      </c>
+      <c r="B23" s="2" t="inlineStr">
+        <is>
+          <t>13:13:57</t>
+        </is>
+      </c>
+      <c r="C23" s="2" t="inlineStr">
+        <is>
+          <t>13:22:56</t>
+        </is>
+      </c>
+      <c r="D23" s="2" t="inlineStr">
+        <is>
+          <t>up</t>
+        </is>
+      </c>
+      <c r="E23" t="n">
+        <v>25962.75</v>
+      </c>
+      <c r="F23" t="n">
+        <v>25958.8</v>
+      </c>
+      <c r="G23" t="n">
+        <v>-3.95</v>
+      </c>
+    </row>
+    <row r="24" ht="15.75" customHeight="1" s="8">
+      <c r="A24" s="2" t="inlineStr">
+        <is>
+          <t>2024-09-24</t>
+        </is>
+      </c>
+      <c r="B24" s="2" t="inlineStr">
+        <is>
+          <t>13:29:45</t>
+        </is>
+      </c>
+      <c r="C24" s="2" t="inlineStr">
+        <is>
+          <t>13:34:22</t>
+        </is>
+      </c>
+      <c r="D24" s="2" t="inlineStr">
+        <is>
+          <t>down</t>
+        </is>
+      </c>
+      <c r="E24" t="n">
+        <v>25958.3</v>
+      </c>
+      <c r="F24" t="n">
+        <v>25961.1</v>
+      </c>
+      <c r="G24" t="n">
+        <v>-2.8</v>
+      </c>
+    </row>
+    <row r="25" ht="15.75" customHeight="1" s="8">
+      <c r="A25" s="2" t="inlineStr">
+        <is>
+          <t>2024-09-24</t>
+        </is>
+      </c>
+      <c r="B25" s="2" t="inlineStr">
+        <is>
+          <t>13:35:05</t>
+        </is>
+      </c>
+      <c r="C25" s="2" t="inlineStr">
+        <is>
+          <t>13:39:44</t>
+        </is>
+      </c>
+      <c r="D25" s="2" t="inlineStr">
+        <is>
+          <t>up</t>
+        </is>
+      </c>
+      <c r="E25" t="n">
+        <v>25966.95</v>
+      </c>
+      <c r="F25" t="n">
+        <v>25960.15</v>
+      </c>
+      <c r="G25" t="n">
+        <v>-6.8</v>
+      </c>
+    </row>
+    <row r="26" ht="15.75" customHeight="1" s="8">
+      <c r="A26" s="2" t="inlineStr">
+        <is>
+          <t>2024-09-24</t>
+        </is>
+      </c>
+      <c r="B26" s="2" t="inlineStr">
+        <is>
+          <t>13:57:14</t>
+        </is>
+      </c>
+      <c r="C26" s="2" t="inlineStr">
+        <is>
+          <t>14:00:59</t>
+        </is>
+      </c>
+      <c r="D26" s="2" t="inlineStr">
+        <is>
+          <t>down</t>
+        </is>
+      </c>
+      <c r="E26" t="n">
+        <v>25964.75</v>
+      </c>
+      <c r="F26" t="n">
+        <v>25970.8</v>
+      </c>
+      <c r="G26" t="n">
+        <v>-6.05</v>
+      </c>
+    </row>
+    <row r="27" ht="15.75" customHeight="1" s="8">
+      <c r="A27" s="2" t="inlineStr">
+        <is>
+          <t>2024-09-24</t>
+        </is>
+      </c>
+      <c r="B27" s="2" t="inlineStr">
+        <is>
+          <t>14:01:42</t>
+        </is>
+      </c>
+      <c r="C27" s="2" t="inlineStr">
+        <is>
+          <t>14:12:03</t>
+        </is>
+      </c>
+      <c r="D27" s="2" t="inlineStr">
+        <is>
+          <t>up</t>
+        </is>
+      </c>
+      <c r="E27" t="n">
+        <v>25974</v>
+      </c>
+      <c r="F27" t="n">
+        <v>25972.5</v>
+      </c>
+      <c r="G27" t="n">
         <v>-1.5</v>
       </c>
     </row>
-    <row r="12" ht="15.75" customHeight="1" s="8">
-      <c r="A12" s="2" t="n"/>
-      <c r="B12" s="2" t="n"/>
-      <c r="C12" s="2" t="n"/>
-      <c r="D12" s="2" t="n"/>
-    </row>
-    <row r="13" ht="15.75" customHeight="1" s="8">
-      <c r="A13" s="2" t="n"/>
-      <c r="B13" s="2" t="n"/>
-      <c r="C13" s="2" t="n"/>
-      <c r="D13" s="2" t="n"/>
-    </row>
-    <row r="14" ht="15.75" customHeight="1" s="8">
-      <c r="A14" s="2" t="n"/>
-      <c r="B14" s="2" t="n"/>
-      <c r="C14" s="2" t="n"/>
-      <c r="D14" s="2" t="n"/>
-    </row>
-    <row r="15" ht="15.75" customHeight="1" s="8">
-      <c r="A15" s="2" t="n"/>
-      <c r="B15" s="2" t="n"/>
-      <c r="C15" s="2" t="n"/>
-      <c r="D15" s="2" t="n"/>
-    </row>
-    <row r="16" ht="15.75" customHeight="1" s="8">
-      <c r="A16" s="2" t="n"/>
-      <c r="B16" s="2" t="n"/>
-      <c r="C16" s="2" t="n"/>
-      <c r="D16" s="2" t="n"/>
-    </row>
-    <row r="17" ht="15.75" customHeight="1" s="8">
-      <c r="A17" s="2" t="n"/>
-      <c r="B17" s="2" t="n"/>
-      <c r="C17" s="2" t="n"/>
-      <c r="D17" s="2" t="n"/>
-    </row>
-    <row r="18" ht="15.75" customHeight="1" s="8">
-      <c r="A18" s="2" t="n"/>
-      <c r="B18" s="2" t="n"/>
-      <c r="C18" s="2" t="n"/>
-      <c r="D18" s="2" t="n"/>
-    </row>
-    <row r="19" ht="15.75" customHeight="1" s="8">
-      <c r="A19" s="2" t="n"/>
-      <c r="B19" s="2" t="n"/>
-      <c r="C19" s="2" t="n"/>
-      <c r="D19" s="2" t="n"/>
-    </row>
-    <row r="20" ht="15.75" customHeight="1" s="8">
-      <c r="A20" s="2" t="n"/>
-      <c r="B20" s="2" t="n"/>
-      <c r="C20" s="2" t="n"/>
-      <c r="D20" s="2" t="n"/>
-    </row>
-    <row r="21" ht="15.75" customHeight="1" s="8">
-      <c r="A21" s="2" t="n"/>
-      <c r="B21" s="2" t="n"/>
-      <c r="C21" s="2" t="n"/>
-      <c r="D21" s="2" t="n"/>
-    </row>
-    <row r="22" ht="15.75" customHeight="1" s="8">
-      <c r="A22" s="2" t="n"/>
-      <c r="B22" s="2" t="n"/>
-      <c r="C22" s="2" t="n"/>
-      <c r="D22" s="2" t="n"/>
-    </row>
-    <row r="23" ht="15.75" customHeight="1" s="8">
-      <c r="A23" s="2" t="n"/>
-      <c r="B23" s="2" t="n"/>
-      <c r="C23" s="2" t="n"/>
-      <c r="D23" s="2" t="n"/>
-    </row>
-    <row r="24" ht="15.75" customHeight="1" s="8">
-      <c r="A24" s="2" t="n"/>
-      <c r="B24" s="2" t="n"/>
-      <c r="C24" s="2" t="n"/>
-      <c r="D24" s="2" t="n"/>
-    </row>
-    <row r="25" ht="15.75" customHeight="1" s="8">
-      <c r="A25" s="2" t="n"/>
-      <c r="B25" s="2" t="n"/>
-      <c r="C25" s="2" t="n"/>
-      <c r="D25" s="2" t="n"/>
-    </row>
-    <row r="26" ht="15.75" customHeight="1" s="8">
-      <c r="A26" s="2" t="n"/>
-      <c r="B26" s="2" t="n"/>
-      <c r="C26" s="2" t="n"/>
-      <c r="D26" s="2" t="n"/>
-    </row>
-    <row r="27" ht="15.75" customHeight="1" s="8">
-      <c r="A27" s="2" t="n"/>
-      <c r="B27" s="2" t="n"/>
-      <c r="C27" s="2" t="n"/>
-      <c r="D27" s="2" t="n"/>
-    </row>
     <row r="28" ht="15.75" customHeight="1" s="8">
-      <c r="A28" s="2" t="n"/>
-      <c r="B28" s="2" t="n"/>
-      <c r="C28" s="2" t="n"/>
-      <c r="D28" s="2" t="n"/>
+      <c r="A28" s="2" t="inlineStr">
+        <is>
+          <t>2024-09-24</t>
+        </is>
+      </c>
+      <c r="B28" s="2" t="inlineStr">
+        <is>
+          <t>14:15:47</t>
+        </is>
+      </c>
+      <c r="C28" s="2" t="inlineStr">
+        <is>
+          <t>14:21:42</t>
+        </is>
+      </c>
+      <c r="D28" s="2" t="inlineStr">
+        <is>
+          <t>up</t>
+        </is>
+      </c>
+      <c r="E28" t="n">
+        <v>25980.75</v>
+      </c>
+      <c r="F28" t="n">
+        <v>25980.3</v>
+      </c>
+      <c r="G28" t="n">
+        <v>-0.45</v>
+      </c>
     </row>
     <row r="29" ht="15.75" customHeight="1" s="8">
-      <c r="A29" s="2" t="n"/>
-      <c r="B29" s="2" t="n"/>
-      <c r="C29" s="2" t="n"/>
-      <c r="D29" s="2" t="n"/>
+      <c r="A29" s="2" t="inlineStr">
+        <is>
+          <t>2024-09-24</t>
+        </is>
+      </c>
+      <c r="B29" s="2" t="inlineStr">
+        <is>
+          <t>14:22:10</t>
+        </is>
+      </c>
+      <c r="C29" s="2" t="inlineStr">
+        <is>
+          <t>14:24:04</t>
+        </is>
+      </c>
+      <c r="D29" s="2" t="inlineStr">
+        <is>
+          <t>down</t>
+        </is>
+      </c>
+      <c r="E29" t="n">
+        <v>25961.45</v>
+      </c>
+      <c r="F29" t="n">
+        <v>25970.7</v>
+      </c>
+      <c r="G29" t="n">
+        <v>-9.25</v>
+      </c>
     </row>
     <row r="30" ht="15.75" customHeight="1" s="8">
-      <c r="A30" s="2" t="n"/>
-      <c r="B30" s="2" t="n"/>
-      <c r="C30" s="2" t="n"/>
-      <c r="D30" s="2" t="n"/>
+      <c r="A30" s="2" t="inlineStr">
+        <is>
+          <t>2024-09-24</t>
+        </is>
+      </c>
+      <c r="B30" s="2" t="inlineStr">
+        <is>
+          <t>14:28:30</t>
+        </is>
+      </c>
+      <c r="C30" s="2" t="inlineStr">
+        <is>
+          <t>14:32:10</t>
+        </is>
+      </c>
+      <c r="D30" s="2" t="inlineStr">
+        <is>
+          <t>down</t>
+        </is>
+      </c>
+      <c r="E30" t="n">
+        <v>25971</v>
+      </c>
+      <c r="F30" t="n">
+        <v>25978.8</v>
+      </c>
+      <c r="G30" t="n">
+        <v>-7.8</v>
+      </c>
     </row>
     <row r="31" ht="15.75" customHeight="1" s="8">
-      <c r="A31" s="2" t="n"/>
-      <c r="B31" s="2" t="n"/>
-      <c r="C31" s="2" t="n"/>
-      <c r="D31" s="2" t="n"/>
+      <c r="A31" s="2" t="inlineStr">
+        <is>
+          <t>2024-09-24</t>
+        </is>
+      </c>
+      <c r="B31" s="2" t="inlineStr">
+        <is>
+          <t>14:38:12</t>
+        </is>
+      </c>
+      <c r="C31" s="2" t="inlineStr">
+        <is>
+          <t>14:43:15</t>
+        </is>
+      </c>
+      <c r="D31" s="2" t="inlineStr">
+        <is>
+          <t>up</t>
+        </is>
+      </c>
+      <c r="E31" t="n">
+        <v>25984.85</v>
+      </c>
+      <c r="F31" t="n">
+        <v>25977.15</v>
+      </c>
+      <c r="G31" t="n">
+        <v>-7.7</v>
+      </c>
     </row>
     <row r="32" ht="15.75" customHeight="1" s="8">
-      <c r="A32" s="2" t="n"/>
-      <c r="B32" s="2" t="n"/>
-      <c r="C32" s="2" t="n"/>
-      <c r="D32" s="2" t="n"/>
+      <c r="A32" s="2" t="inlineStr">
+        <is>
+          <t>2024-09-24</t>
+        </is>
+      </c>
+      <c r="B32" s="2" t="inlineStr">
+        <is>
+          <t>14:43:47</t>
+        </is>
+      </c>
+      <c r="C32" s="2" t="inlineStr">
+        <is>
+          <t>14:44:59</t>
+        </is>
+      </c>
+      <c r="D32" s="2" t="inlineStr">
+        <is>
+          <t>down</t>
+        </is>
+      </c>
+      <c r="E32" t="n">
+        <v>25975.5</v>
+      </c>
+      <c r="F32" t="n">
+        <v>25979.45</v>
+      </c>
+      <c r="G32" t="n">
+        <v>-3.95</v>
+      </c>
     </row>
     <row r="33" ht="15.75" customHeight="1" s="8">
       <c r="A33" s="2" t="n"/>

</xml_diff>